<commit_message>
changed for Feb 2018 updates including product_collection in line item properties
</commit_message>
<xml_diff>
--- a/current_products.xlsx
+++ b/current_products.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>prod_id_key</t>
   </si>
@@ -55,12 +55,54 @@
   </si>
   <si>
     <t>go_time5_auto2</t>
+  </si>
+  <si>
+    <t>heart_soul_3item</t>
+  </si>
+  <si>
+    <t>heart_soul_3item_auto</t>
+  </si>
+  <si>
+    <t>heart_soul_5item</t>
+  </si>
+  <si>
+    <t>heart_soul_5item_auto</t>
+  </si>
+  <si>
+    <t>go_time_3item</t>
+  </si>
+  <si>
+    <t>fit_fierce_5item</t>
+  </si>
+  <si>
+    <t>modern_muse_5itemauto</t>
+  </si>
+  <si>
+    <t>power_move_3_item</t>
+  </si>
+  <si>
+    <t>fit_fierce_3item</t>
+  </si>
+  <si>
+    <t>modern_muse_3item</t>
+  </si>
+  <si>
+    <t>modern_muse_5item</t>
+  </si>
+  <si>
+    <t>fit_fierce_3itemauto</t>
+  </si>
+  <si>
+    <t>modern_muse_3itemauto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="###########00000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -109,7 +151,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -117,18 +159,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,17 +521,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C21" sqref="C21:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -486,100 +549,247 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>69026938898</v>
       </c>
-      <c r="C2" s="1">
-        <v>91236171794</v>
+      <c r="C2" s="2">
+        <v>138427301906</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>69026316306</v>
       </c>
-      <c r="C3">
-        <v>91235975186</v>
+      <c r="C3" s="1">
+        <v>138427203602</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>52386937778</v>
       </c>
-      <c r="C4" s="1">
-        <v>91236171794</v>
+      <c r="C4" s="2">
+        <v>138427301906</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>78480408594</v>
       </c>
-      <c r="C5">
-        <v>91235975186</v>
+      <c r="C5" s="1">
+        <v>138427203602</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>78541520914</v>
       </c>
-      <c r="C6" s="1">
-        <v>91236171794</v>
+      <c r="C6" s="2">
+        <v>138427301906</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>78657093650</v>
       </c>
-      <c r="C7">
-        <v>91235975186</v>
+      <c r="C7" s="1">
+        <v>138427203602</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>91049066514</v>
       </c>
-      <c r="C8" s="1">
-        <v>91236171794</v>
+      <c r="C8" s="2">
+        <v>138427301906</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>91049230354</v>
       </c>
-      <c r="C9">
-        <v>91235975186</v>
+      <c r="C9" s="1">
+        <v>138427203602</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>91049197586</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
+        <v>138427203602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>91236466706</v>
+      </c>
+      <c r="C11" s="2">
+        <v>138427301906</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>109303332882</v>
+      </c>
+      <c r="C12" s="2">
+        <v>138427301906</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>109301366802</v>
+      </c>
+      <c r="C13" s="1">
+        <v>138427203602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>109301366802</v>
+      </c>
+      <c r="C14" s="1">
+        <v>138427203602</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>52386037778</v>
+      </c>
+      <c r="C15" s="2">
+        <v>138427301906</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
         <v>91235975186</v>
       </c>
+      <c r="C16" s="1">
+        <v>138427203602</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1">
+        <v>91236368402</v>
+      </c>
+      <c r="C17" s="1">
+        <v>138427203602</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1">
+        <v>69026938898</v>
+      </c>
+      <c r="C18" s="2">
+        <v>138427301906</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1">
+        <v>91236171794</v>
+      </c>
+      <c r="C19" s="2">
+        <v>138427301906</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>91236368402</v>
+      </c>
+      <c r="C20" s="1">
+        <v>138427203602</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1">
+        <v>91236466706</v>
+      </c>
+      <c r="C21" s="2">
+        <v>138427301906</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1">
+        <v>91236171794</v>
+      </c>
+      <c r="C22" s="2">
+        <v>138427301906</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1">
+        <v>91236466706</v>
+      </c>
+      <c r="C23" s="2">
+        <v>138427301906</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>